<commit_message>
20XWO8: Complete Batch1 Practice3
</commit_message>
<xml_diff>
--- a/20XWO8 - DATA VISUALIZATION/Practice3/Practice3.xlsx
+++ b/20XWO8 - DATA VISUALIZATION/Practice3/Practice3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\college8\20XWO8 - DATA VISUALIZATION\Practice3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6A371-BE63-4A54-833C-4449B0FBD81B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230660CA-84FB-40DF-81F3-D9E750A4A545}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Jenny</t>
+  </si>
+  <si>
+    <t>UNIT TEST</t>
+  </si>
+  <si>
+    <t>MIDTERM TEST</t>
+  </si>
+  <si>
+    <t>FINAL TEST</t>
+  </si>
+  <si>
+    <t>UNITTEST</t>
   </si>
 </sst>
 </file>
@@ -117,14 +129,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,338 +424,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>38</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>58</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>66</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>88</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>92</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>74</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5">
+        <f>VLOOKUP(G4, IF(H2="UNITTEST",$A$3:$E$7,IF(H2="MIDTERMTEST",$A$11:$E$15,$A$19:$E$23)),MATCH(H3,$A$2:$E$2,0),0)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>57</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>77</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>91</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E5" s="1">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>82</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>56</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>45</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>55</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>55</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>65</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B11" s="1">
         <v>71</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="1">
         <v>41</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D11" s="1">
         <v>50</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E11" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="1">
         <v>86</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>91</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D12" s="1">
         <v>41</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E12" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B13" s="1">
         <v>41</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="1">
         <v>66</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="1">
         <v>85</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E13" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B14" s="1">
         <v>45</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C14" s="1">
         <v>53</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D14" s="1">
         <v>76</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E14" s="1">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B15" s="1">
         <v>63</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="1">
         <v>73</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D15" s="1">
         <v>68</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E15" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1">
-        <v>51</v>
-      </c>
-      <c r="C16" s="1">
-        <v>83</v>
-      </c>
-      <c r="D16" s="1">
-        <v>80</v>
-      </c>
-      <c r="E16" s="1">
-        <v>50</v>
-      </c>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1">
-        <v>74</v>
-      </c>
-      <c r="C17" s="1">
-        <v>46</v>
-      </c>
-      <c r="D17" s="1">
-        <v>58</v>
-      </c>
-      <c r="E17" s="1">
-        <v>51</v>
-      </c>
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1">
-        <v>89</v>
-      </c>
-      <c r="C18" s="1">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1">
-        <v>59</v>
-      </c>
-      <c r="E18" s="1">
-        <v>53</v>
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1">
+        <v>58</v>
+      </c>
+      <c r="E20" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>89</v>
+      </c>
+      <c r="C21" s="1">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1">
+        <v>59</v>
+      </c>
+      <c r="E21" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1">
+        <v>48</v>
+      </c>
+      <c r="E22" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B23" s="1">
         <v>50</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C23" s="1">
         <v>64</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D23" s="1">
         <v>50</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E23" s="1">
         <v>75</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A17:E17"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{9547DA55-05F0-4308-ABAB-30EF7A783677}">
+      <formula1>"UNITTEST, MIDTERMTEST, FINALTEST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3" xr:uid="{ADE5655D-E92A-40EA-9F41-D75A8D438E88}">
+      <formula1>$B$2:$E$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{074EC623-AE80-4E28-9A43-3852ADA8BA4A}">
+      <formula1>$A$3:$A$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>